<commit_message>
prepare for GetVersionList api
</commit_message>
<xml_diff>
--- a/cfg/schema/systems.xlsx
+++ b/cfg/schema/systems.xlsx
@@ -123,10 +123,10 @@
     <t>游戏系统配置</t>
   </si>
   <si>
-    <t>game_system_test</t>
-  </si>
-  <si>
     <t>gameAdmin2</t>
+  </si>
+  <si>
+    <t>test_game_system</t>
   </si>
 </sst>
 </file>
@@ -657,7 +657,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -668,7 +668,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
@@ -704,13 +704,13 @@
     </row>
     <row r="2" spans="1:6" ht="13.5" customHeight="1">
       <c r="A2" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>22</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
new database 'test_game_logDB' and new table 'T_MON_SERVICE'
</commit_message>
<xml_diff>
--- a/cfg/schema/systems.xlsx
+++ b/cfg/schema/systems.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="900" windowWidth="25340" windowHeight="9600"/>
+    <workbookView xWindow="11480" yWindow="4040" windowWidth="25340" windowHeight="9600"/>
   </bookViews>
   <sheets>
     <sheet name="Database" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -127,6 +127,26 @@
   </si>
   <si>
     <t>test_game_system</t>
+  </si>
+  <si>
+    <t>test_game_logDB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>localhost</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gameAdmin2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>game_log</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>游戏log</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -137,14 +157,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -152,14 +172,14 @@
     <font>
       <sz val="9"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -168,7 +188,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -177,7 +197,7 @@
       <u/>
       <sz val="11"/>
       <color theme="11"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -190,7 +210,7 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -309,17 +329,17 @@
     </xf>
   </cellXfs>
   <cellStyles count="11">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -657,7 +677,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -665,10 +685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
@@ -720,6 +740,26 @@
       </c>
       <c r="F2" s="9" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="13.5" customHeight="1">
+      <c r="A3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>